<commit_message>
added ability to read into Map
</commit_message>
<xml_diff>
--- a/src/main/resources/test.xlsx
+++ b/src/main/resources/test.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Urban Space 100</t>
   </si>
   <si>
     <t xml:space="preserve">Name 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nam1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nam2</t>
   </si>
   <si>
     <t xml:space="preserve">Name 2</t>
@@ -128,7 +134,7 @@
   <dimension ref="B2:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -186,12 +192,24 @@
       <c r="C11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add nested class ability for Map interface
</commit_message>
<xml_diff>
--- a/src/main/resources/test.xlsx
+++ b/src/main/resources/test.xlsx
@@ -20,21 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Urban Space 100</t>
   </si>
   <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Nam1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nam2</t>
+    <t xml:space="preserve">2e</t>
   </si>
   <si>
     <t xml:space="preserve">Name 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3a</t>
   </si>
 </sst>
 </file>
@@ -134,7 +146,7 @@
   <dimension ref="B2:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -185,32 +197,58 @@
         <v>4</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first test cases & refactoring the main logic
</commit_message>
<xml_diff>
--- a/src/main/resources/test.xlsx
+++ b/src/main/resources/test.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="position" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,41 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">Urban Space 100</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3a</t>
+    <t xml:space="preserve">name2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -121,8 +101,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -143,10 +127,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:I12"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -156,99 +140,37 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>123</v>
+      <c r="C1" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D1" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
-        <v>3</v>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="n">
-        <v>4</v>
+      <c r="A5" s="0" t="n">
+        <v>2</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>2</v>
+      <c r="C5" s="0" t="n">
+        <v>21.3</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>6</v>
+      <c r="D5" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>